<commit_message>
Fix typo with namespaces and xsl:output.
</commit_message>
<xml_diff>
--- a/xml-vs-json/Comparison.xlsx
+++ b/xml-vs-json/Comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\Source\Prague2016\xml-vs-json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AF97B9-59FC-47EF-86FC-4CCC0961DE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF13B3A8-3FDC-467D-ADCD-96BFC1D79183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" activeTab="1" xr2:uid="{2CD50D15-792B-4B03-8967-94A030FF404F}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{2CD50D15-792B-4B03-8967-94A030FF404F}"/>
   </bookViews>
   <sheets>
     <sheet name="Courses" sheetId="1" r:id="rId1"/>
@@ -359,34 +359,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4.777749</c:v>
+                  <c:v>5.9041160000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.7023999999999999</c:v>
+                  <c:v>6.4622999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.1535159999999998</c:v>
+                  <c:v>7.7937500000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.2694320000000001</c:v>
+                  <c:v>8.7020999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.0320989999999997</c:v>
+                  <c:v>9.1550829999999994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.603866</c:v>
+                  <c:v>12.400766000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.3884000000000007</c:v>
+                  <c:v>22.224381999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18.046316000000001</c:v>
+                  <c:v>37.048099999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32.270783000000002</c:v>
+                  <c:v>54.853316</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>34.554349999999999</c:v>
+                  <c:v>139.180566</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2609,8 +2609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535B11A5-85F1-40E1-857F-89A9A0BFE57B}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" activeCellId="2" sqref="A1:A1048576 B1:B1048576 C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2634,7 +2634,7 @@
         <v>5.0237499999999997</v>
       </c>
       <c r="C2">
-        <v>4.777749</v>
+        <v>5.9041160000000001</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.75">
@@ -2645,7 +2645,7 @@
         <v>6.023333</v>
       </c>
       <c r="C3">
-        <v>3.7023999999999999</v>
+        <v>6.4622999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.75">
@@ -2656,7 +2656,7 @@
         <v>7.0720999999999998</v>
       </c>
       <c r="C4">
-        <v>4.1535159999999998</v>
+        <v>7.7937500000000002</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.75">
@@ -2667,7 +2667,7 @@
         <v>7.855283</v>
       </c>
       <c r="C5">
-        <v>4.2694320000000001</v>
+        <v>8.7020999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.75">
@@ -2678,7 +2678,7 @@
         <v>13.035083</v>
       </c>
       <c r="C6">
-        <v>7.0320989999999997</v>
+        <v>9.1550829999999994</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.75">
@@ -2689,7 +2689,7 @@
         <v>21.310549999999999</v>
       </c>
       <c r="C7">
-        <v>9.603866</v>
+        <v>12.400766000000001</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.75">
@@ -2700,7 +2700,7 @@
         <v>25.366849999999999</v>
       </c>
       <c r="C8">
-        <v>9.3884000000000007</v>
+        <v>22.224381999999999</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.75">
@@ -2711,7 +2711,7 @@
         <v>53.742365999999997</v>
       </c>
       <c r="C9">
-        <v>18.046316000000001</v>
+        <v>37.048099999999998</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.75">
@@ -2722,7 +2722,7 @@
         <v>86.562849999999997</v>
       </c>
       <c r="C10">
-        <v>32.270783000000002</v>
+        <v>54.853316</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.75">
@@ -2733,7 +2733,7 @@
         <v>148.47099900000001</v>
       </c>
       <c r="C11">
-        <v>34.554349999999999</v>
+        <v>139.180566</v>
       </c>
     </row>
   </sheetData>
@@ -2747,7 +2747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{516182E0-9AAB-4ADD-AC35-66CAE6B3D472}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" activeCellId="2" sqref="A1:A1048576 B1:B1048576 C1:C1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>